<commit_message>
Update: - Quyền view có thể print - Tạo thêm 04 Forms in theo mẫu Song Ngữ
</commit_message>
<xml_diff>
--- a/EMR/EMR_Doc.xlsx
+++ b/EMR/EMR_Doc.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aih\AIH Project\EMR_PRO\CLIENT\EMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5596CE-BB89-4B0D-9F45-7A76D953CB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A60496-BBC1-4D95-8347-7F7F69FEB6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B6E0B764-DFA9-4C42-B9D1-92DA6DF13038}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
     <sheet name="Settings" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
-    <sheet name="Permission" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Permission" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>8f06c646-c660-43c1-ad9f-133792acf2b2</t>
   </si>
@@ -114,15 +115,6 @@
     <t>v21</t>
   </si>
   <si>
-    <t>Forms</t>
-  </si>
-  <si>
-    <t>VS Free Text</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>Delete Form Final</t>
   </si>
   <si>
@@ -160,13 +152,41 @@
   </si>
   <si>
     <t>OUTPATIENT MEDICAL RECORD</t>
+  </si>
+  <si>
+    <t>Chưa update api PRO</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Updating</t>
+  </si>
+  <si>
+    <t>OutPatMedRecPed</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>- allow input value vital signs
+- new vaccination field</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>ALLOW_ADD_MUL_DOC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +204,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,9 +237,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,10 +562,13 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -549,6 +583,9 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
       <c r="M1" t="s">
         <v>14</v>
       </c>
@@ -557,11 +594,11 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
@@ -574,8 +611,8 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="F3" t="s">
+        <v>40</v>
       </c>
       <c r="M3" t="s">
         <v>4</v>
@@ -625,7 +662,7 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="M6" t="s">
@@ -636,6 +673,9 @@
       <c r="A7" t="s">
         <v>19</v>
       </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -679,16 +719,19 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
       <c r="M10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -700,14 +743,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{F82EDF89-BF15-4FFC-BA18-B236E1BBE4C9}">
       <formula1>$C$3:$M$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{9802E3D3-19CA-48AF-A415-36B90DB8C1A3}">
-      <formula1>$C$4:$M$4</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{73C4B582-BBB7-4986-8720-9456EDBDFCC4}">
       <formula1>$C$5:$M$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{294C36C2-A2C2-494F-B7B6-C78B8FC7C8DF}">
-      <formula1>$C$2:$M$2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{4EAA12CC-5CC3-4532-9182-1A5BB0ECC59E}">
       <formula1>$C$6:$M$6</formula1>
@@ -721,8 +758,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{FC5BA4A9-96F2-4F57-9CB0-D55145CC5591}">
       <formula1>$C$9:$M$9</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{9802E3D3-19CA-48AF-A415-36B90DB8C1A3}">
+      <formula1>$C$4:$M$4</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{06CAC842-29F3-4E05-A080-4056A16A7D94}">
       <formula1>$C$10:$L$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{294C36C2-A2C2-494F-B7B6-C78B8FC7C8DF}">
+      <formula1>$D$2:$M$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -732,35 +775,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63362E98-6580-4306-B20F-0D8E27F2354E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C5" t="b">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="B1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -770,6 +798,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7485179F-4525-4840-9B71-E06B565C5F3E}">
+  <dimension ref="B2:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872B1240-7AE7-4D8D-9A22-F0CF81933548}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -805,72 +870,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9BBF0E-B9E0-4C7C-8FF1-7E311BDA39FE}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -878,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>